<commit_message>
update clear cached data
</commit_message>
<xml_diff>
--- a/crassets.xlsx
+++ b/crassets.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="42">
   <si>
     <t>Name</t>
   </si>
@@ -153,6 +153,9 @@
   </si>
   <si>
     <t>Storage</t>
+  </si>
+  <si>
+    <t>STORJ</t>
   </si>
 </sst>
 </file>
@@ -470,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -873,6 +876,20 @@
         <v>10</v>
       </c>
     </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29">
+        <v>1649</v>
+      </c>
+      <c r="C29">
+        <v>0.65800000000000003</v>
+      </c>
+      <c r="D29" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
port for displying the app
</commit_message>
<xml_diff>
--- a/crassets.xlsx
+++ b/crassets.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="41">
   <si>
     <t>Name</t>
   </si>
@@ -81,9 +81,6 @@
   </si>
   <si>
     <t>Layer 2</t>
-  </si>
-  <si>
-    <t>ADA</t>
   </si>
   <si>
     <t>ONT</t>
@@ -473,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,10 +528,10 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>33.54</v>
+        <v>42.31</v>
       </c>
       <c r="C4">
-        <v>21</v>
+        <v>37.380000000000003</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -559,7 +556,7 @@
         <v>11</v>
       </c>
       <c r="B6">
-        <v>1481</v>
+        <v>1488</v>
       </c>
       <c r="C6">
         <v>7</v>
@@ -615,13 +612,13 @@
         <v>17</v>
       </c>
       <c r="B10">
-        <v>1639.4</v>
+        <v>1643</v>
       </c>
       <c r="C10">
-        <v>1.5</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D10" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -629,41 +626,41 @@
         <v>18</v>
       </c>
       <c r="B11">
-        <v>1643</v>
+        <v>49.1</v>
       </c>
       <c r="C11">
-        <v>1.1000000000000001</v>
+        <v>66.3</v>
       </c>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B12">
-        <v>49.1</v>
+        <v>5746.13</v>
       </c>
       <c r="C12">
-        <v>66.3</v>
+        <v>0.35099999999999998</v>
       </c>
       <c r="D12" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13">
+        <v>9257.4</v>
+      </c>
+      <c r="C13">
+        <v>0.21</v>
+      </c>
+      <c r="D13" t="s">
         <v>21</v>
-      </c>
-      <c r="B13">
-        <v>5746.13</v>
-      </c>
-      <c r="C13">
-        <v>0.35099999999999998</v>
-      </c>
-      <c r="D13" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -671,13 +668,13 @@
         <v>23</v>
       </c>
       <c r="B14">
-        <v>9257.4</v>
+        <v>7434.88</v>
       </c>
       <c r="C14">
-        <v>0.21</v>
+        <v>0.33900000000000002</v>
       </c>
       <c r="D14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -685,69 +682,69 @@
         <v>24</v>
       </c>
       <c r="B15">
-        <v>7434.88</v>
+        <v>364.1</v>
       </c>
       <c r="C15">
-        <v>0.33900000000000002</v>
+        <v>4.4240000000000004</v>
       </c>
       <c r="D15" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B16">
-        <v>364.1</v>
+        <v>1182.2</v>
       </c>
       <c r="C16">
-        <v>4.4240000000000004</v>
+        <v>2.85</v>
       </c>
       <c r="D16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17">
+        <v>56453.4</v>
+      </c>
+      <c r="C17">
+        <v>0.08</v>
+      </c>
+      <c r="D17" t="s">
         <v>27</v>
-      </c>
-      <c r="B17">
-        <v>1182.2</v>
-      </c>
-      <c r="C17">
-        <v>2.85</v>
-      </c>
-      <c r="D17" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="B18">
-        <v>56453.4</v>
+        <v>98.07</v>
       </c>
       <c r="C18">
-        <v>0.08</v>
+        <v>8.0860000000000003</v>
       </c>
       <c r="D18" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B19">
-        <v>98.07</v>
+        <v>11.042</v>
       </c>
       <c r="C19">
-        <v>8.0860000000000003</v>
+        <v>97.25</v>
       </c>
       <c r="D19" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -755,13 +752,13 @@
         <v>30</v>
       </c>
       <c r="B20">
-        <v>11.042</v>
+        <v>180.5</v>
       </c>
       <c r="C20">
-        <v>97.25</v>
+        <v>7.2</v>
       </c>
       <c r="D20" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -769,13 +766,13 @@
         <v>31</v>
       </c>
       <c r="B21">
-        <v>180.5</v>
+        <v>228</v>
       </c>
       <c r="C21">
-        <v>7.2</v>
+        <v>0.49399999999999999</v>
       </c>
       <c r="D21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -783,13 +780,13 @@
         <v>32</v>
       </c>
       <c r="B22">
-        <v>228</v>
+        <v>3618.3</v>
       </c>
       <c r="C22">
-        <v>0.49399999999999999</v>
+        <v>0.12</v>
       </c>
       <c r="D22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -797,13 +794,13 @@
         <v>33</v>
       </c>
       <c r="B23">
-        <v>3618.3</v>
+        <v>105.44</v>
       </c>
       <c r="C23">
-        <v>0.12</v>
+        <v>9</v>
       </c>
       <c r="D23" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -811,13 +808,13 @@
         <v>34</v>
       </c>
       <c r="B24">
-        <v>105.44</v>
+        <v>96.5</v>
       </c>
       <c r="C24">
-        <v>9</v>
+        <v>2.88</v>
       </c>
       <c r="D24" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -825,13 +822,13 @@
         <v>35</v>
       </c>
       <c r="B25">
-        <v>96.5</v>
+        <v>22.74</v>
       </c>
       <c r="C25">
-        <v>2.88</v>
+        <v>44</v>
       </c>
       <c r="D25" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -839,13 +836,13 @@
         <v>36</v>
       </c>
       <c r="B26">
-        <v>22.74</v>
+        <v>2667</v>
       </c>
       <c r="C26">
-        <v>44</v>
+        <v>0.68</v>
       </c>
       <c r="D26" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -853,40 +850,26 @@
         <v>37</v>
       </c>
       <c r="B27">
-        <v>2667</v>
+        <v>441238</v>
       </c>
       <c r="C27">
-        <v>0.68</v>
+        <v>2.5500000000000002E-3</v>
       </c>
       <c r="D27" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B28">
-        <v>441238</v>
+        <v>1191.8</v>
       </c>
       <c r="C28">
-        <v>2.5500000000000002E-3</v>
+        <v>0.86</v>
       </c>
       <c r="D28" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>41</v>
-      </c>
-      <c r="B29">
-        <v>1191.8</v>
-      </c>
-      <c r="C29">
-        <v>0.86</v>
-      </c>
-      <c r="D29" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ohcl plot volume ema5 added
</commit_message>
<xml_diff>
--- a/crassets.xlsx
+++ b/crassets.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -473,15 +473,15 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -495,7 +495,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -509,7 +509,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -523,7 +523,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -531,13 +531,13 @@
         <v>42.31</v>
       </c>
       <c r="C4">
-        <v>37.380000000000003</v>
+        <v>40</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -551,7 +551,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -559,13 +559,13 @@
         <v>1488</v>
       </c>
       <c r="C6">
-        <v>7</v>
+        <v>7.5</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -579,7 +579,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -593,7 +593,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -607,7 +607,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -621,7 +621,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -635,7 +635,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -649,7 +649,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -663,7 +663,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -677,7 +677,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -691,7 +691,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -705,7 +705,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -719,7 +719,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -733,7 +733,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -747,7 +747,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -761,7 +761,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -775,7 +775,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -789,7 +789,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>33</v>
       </c>
@@ -803,7 +803,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>34</v>
       </c>
@@ -817,7 +817,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -831,7 +831,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>36</v>
       </c>
@@ -845,7 +845,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>37</v>
       </c>
@@ -859,7 +859,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>40</v>
       </c>

</xml_diff>

<commit_message>
progress bar bug solved
</commit_message>
<xml_diff>
--- a/crassets.xlsx
+++ b/crassets.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
   <si>
     <t>Name</t>
   </si>
@@ -89,9 +89,6 @@
     <t>AAVE</t>
   </si>
   <si>
-    <t>DeFi</t>
-  </si>
-  <si>
     <t>OCEAN</t>
   </si>
   <si>
@@ -101,9 +98,6 @@
     <t>FET</t>
   </si>
   <si>
-    <t>AGIX</t>
-  </si>
-  <si>
     <t>PYR</t>
   </si>
   <si>
@@ -122,21 +116,12 @@
     <t>ILV</t>
   </si>
   <si>
-    <t>APE</t>
-  </si>
-  <si>
     <t>AGLD</t>
   </si>
   <si>
-    <t>TLM</t>
-  </si>
-  <si>
     <t>API3</t>
   </si>
   <si>
-    <t>SAND</t>
-  </si>
-  <si>
     <t>TRB</t>
   </si>
   <si>
@@ -153,6 +138,15 @@
   </si>
   <si>
     <t>POWR</t>
+  </si>
+  <si>
+    <t>PHB</t>
+  </si>
+  <si>
+    <t>DESO</t>
+  </si>
+  <si>
+    <t>DeFi/So</t>
   </si>
 </sst>
 </file>
@@ -470,18 +464,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A27" sqref="A27:XFD37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -495,7 +489,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -509,7 +503,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -523,7 +517,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -537,7 +531,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -551,7 +545,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -559,13 +553,13 @@
         <v>1488</v>
       </c>
       <c r="C6">
-        <v>7.5</v>
+        <v>8.5</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -579,7 +573,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -593,7 +587,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -607,7 +601,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -621,7 +615,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -632,12 +626,12 @@
         <v>66.3</v>
       </c>
       <c r="D11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>20</v>
       </c>
       <c r="B12">
         <v>5746.13</v>
@@ -646,231 +640,203 @@
         <v>0.35099999999999998</v>
       </c>
       <c r="D12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13">
+        <v>10890</v>
+      </c>
+      <c r="C13">
+        <v>0.375</v>
+      </c>
+      <c r="D13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>22</v>
       </c>
-      <c r="B13">
-        <v>9257.4</v>
-      </c>
-      <c r="C13">
-        <v>0.21</v>
-      </c>
-      <c r="D13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="B14">
+        <v>364.1</v>
+      </c>
+      <c r="C14">
+        <v>4.4240000000000004</v>
+      </c>
+      <c r="D14" t="s">
         <v>23</v>
       </c>
-      <c r="B14">
-        <v>7434.88</v>
-      </c>
-      <c r="C14">
-        <v>0.33900000000000002</v>
-      </c>
-      <c r="D14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>24</v>
       </c>
       <c r="B15">
-        <v>364.1</v>
+        <v>1182.2</v>
       </c>
       <c r="C15">
-        <v>4.4240000000000004</v>
+        <v>2.85</v>
       </c>
       <c r="D15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>26</v>
       </c>
       <c r="B16">
-        <v>1182.2</v>
+        <v>56453.4</v>
       </c>
       <c r="C16">
-        <v>2.85</v>
+        <v>0.08</v>
       </c>
       <c r="D16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17">
+        <v>98.07</v>
+      </c>
+      <c r="C17">
+        <v>8.0860000000000003</v>
+      </c>
+      <c r="D17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="B18">
+        <v>11.042</v>
+      </c>
+      <c r="C18">
+        <v>97.25</v>
+      </c>
+      <c r="D18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>28</v>
       </c>
-      <c r="B17">
-        <v>56453.4</v>
-      </c>
-      <c r="C17">
-        <v>0.08</v>
-      </c>
-      <c r="D17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18">
-        <v>98.07</v>
-      </c>
-      <c r="C18">
-        <v>8.0860000000000003</v>
-      </c>
-      <c r="D18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="B19">
+        <v>228</v>
+      </c>
+      <c r="C19">
+        <v>0.49399999999999999</v>
+      </c>
+      <c r="D19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>29</v>
       </c>
-      <c r="B19">
-        <v>11.042</v>
-      </c>
-      <c r="C19">
-        <v>97.25</v>
-      </c>
-      <c r="D19" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="B20">
+        <v>105.44</v>
+      </c>
+      <c r="C20">
+        <v>9</v>
+      </c>
+      <c r="D20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>30</v>
       </c>
-      <c r="B20">
-        <v>180.5</v>
-      </c>
-      <c r="C20">
-        <v>7.2</v>
-      </c>
-      <c r="D20" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="B21">
+        <v>22.74</v>
+      </c>
+      <c r="C21">
+        <v>44</v>
+      </c>
+      <c r="D21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>31</v>
       </c>
-      <c r="B21">
-        <v>228</v>
-      </c>
-      <c r="C21">
-        <v>0.49399999999999999</v>
-      </c>
-      <c r="D21" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>32</v>
-      </c>
       <c r="B22">
-        <v>3618.3</v>
+        <v>2667</v>
       </c>
       <c r="C22">
-        <v>0.12</v>
+        <v>0.68</v>
       </c>
       <c r="D22" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B23">
-        <v>105.44</v>
+        <v>441238</v>
       </c>
       <c r="C23">
-        <v>9</v>
+        <v>2.5500000000000002E-3</v>
       </c>
       <c r="D23" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B24">
-        <v>96.5</v>
+        <v>1191.8</v>
       </c>
       <c r="C24">
-        <v>2.88</v>
+        <v>0.86</v>
       </c>
       <c r="D24" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B25">
-        <v>22.74</v>
+        <v>2341.8000000000002</v>
       </c>
       <c r="C25">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B26">
-        <v>2667</v>
+        <v>42.56</v>
       </c>
       <c r="C26">
-        <v>0.68</v>
+        <v>46</v>
       </c>
       <c r="D26" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>37</v>
-      </c>
-      <c r="B27">
-        <v>441238</v>
-      </c>
-      <c r="C27">
-        <v>2.5500000000000002E-3</v>
-      </c>
-      <c r="D27" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>40</v>
-      </c>
-      <c r="B28">
-        <v>1191.8</v>
-      </c>
-      <c r="C28">
-        <v>0.86</v>
-      </c>
-      <c r="D28" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor change for crypto name
</commit_message>
<xml_diff>
--- a/crassets.xlsx
+++ b/crassets.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
   <si>
     <t>Name</t>
   </si>
@@ -147,6 +147,9 @@
   </si>
   <si>
     <t>DeFi/So</t>
+  </si>
+  <si>
+    <t>PRIME</t>
   </si>
 </sst>
 </file>
@@ -464,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:XFD37"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -839,6 +842,20 @@
         <v>38</v>
       </c>
     </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27">
+        <v>68.66</v>
+      </c>
+      <c r="C27">
+        <v>8</v>
+      </c>
+      <c r="D27" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
new symbol TIA22861-USD added
</commit_message>
<xml_diff>
--- a/crassets.xlsx
+++ b/crassets.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="43">
   <si>
     <t>Name</t>
   </si>
@@ -150,6 +150,15 @@
   </si>
   <si>
     <t>PRIME</t>
+  </si>
+  <si>
+    <t>OSMO</t>
+  </si>
+  <si>
+    <t>TIA</t>
+  </si>
+  <si>
+    <t>AGIX</t>
   </si>
 </sst>
 </file>
@@ -467,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,7 +562,7 @@
         <v>11</v>
       </c>
       <c r="B6">
-        <v>1488</v>
+        <v>1393</v>
       </c>
       <c r="C6">
         <v>8.5</v>
@@ -854,6 +863,48 @@
       </c>
       <c r="D27" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28">
+        <v>621</v>
+      </c>
+      <c r="C28">
+        <v>1.7</v>
+      </c>
+      <c r="D28" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29">
+        <v>27.5</v>
+      </c>
+      <c r="C29">
+        <v>19</v>
+      </c>
+      <c r="D29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30">
+        <v>1232</v>
+      </c>
+      <c r="C30">
+        <v>0.435</v>
+      </c>
+      <c r="D30" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed problem with min values in plot_port_assetcat
</commit_message>
<xml_diff>
--- a/crassets.xlsx
+++ b/crassets.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="47">
   <si>
     <t>Name</t>
   </si>
@@ -110,12 +110,6 @@
     <t>Metaverse</t>
   </si>
   <si>
-    <t>TVK</t>
-  </si>
-  <si>
-    <t>ILV</t>
-  </si>
-  <si>
     <t>AGLD</t>
   </si>
   <si>
@@ -131,9 +125,6 @@
     <t>VTHO</t>
   </si>
   <si>
-    <t>FIL</t>
-  </si>
-  <si>
     <t>Storage</t>
   </si>
   <si>
@@ -146,9 +137,6 @@
     <t>DESO</t>
   </si>
   <si>
-    <t>DeFi/So</t>
-  </si>
-  <si>
     <t>PRIME</t>
   </si>
   <si>
@@ -159,6 +147,30 @@
   </si>
   <si>
     <t>AGIX</t>
+  </si>
+  <si>
+    <t>INJ</t>
+  </si>
+  <si>
+    <t>DeFi</t>
+  </si>
+  <si>
+    <t>DeSo</t>
+  </si>
+  <si>
+    <t>KUJI</t>
+  </si>
+  <si>
+    <t>VANRY</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>MDT</t>
+  </si>
+  <si>
+    <t>FORT</t>
   </si>
 </sst>
 </file>
@@ -476,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,7 +560,7 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>196842</v>
+        <v>186842</v>
       </c>
       <c r="C5">
         <v>2.1100000000000001E-2</v>
@@ -562,7 +574,7 @@
         <v>11</v>
       </c>
       <c r="B6">
-        <v>1393</v>
+        <v>1239.5999999999999</v>
       </c>
       <c r="C6">
         <v>8.5</v>
@@ -638,7 +650,7 @@
         <v>66.3</v>
       </c>
       <c r="D11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -652,7 +664,7 @@
         <v>0.35099999999999998</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -699,10 +711,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B16">
-        <v>56453.4</v>
+        <v>56240</v>
       </c>
       <c r="C16">
         <v>0.08</v>
@@ -713,27 +725,27 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="B17">
-        <v>98.07</v>
+        <v>27.14</v>
       </c>
       <c r="C17">
-        <v>8.0860000000000003</v>
+        <v>31</v>
       </c>
       <c r="D17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18">
-        <v>11.042</v>
+        <v>228</v>
       </c>
       <c r="C18">
-        <v>97.25</v>
+        <v>0.49399999999999999</v>
       </c>
       <c r="D18" t="s">
         <v>23</v>
@@ -741,27 +753,27 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19">
-        <v>228</v>
+        <v>105.44</v>
       </c>
       <c r="C19">
-        <v>0.49399999999999999</v>
+        <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B20">
-        <v>105.44</v>
+        <v>22.74</v>
       </c>
       <c r="C20">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="D20" t="s">
         <v>13</v>
@@ -769,30 +781,30 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21">
-        <v>22.74</v>
+        <v>2667</v>
       </c>
       <c r="C21">
-        <v>44</v>
+        <v>0.68</v>
       </c>
       <c r="D21" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B22">
-        <v>2667</v>
+        <v>441238</v>
       </c>
       <c r="C22">
-        <v>0.68</v>
+        <v>2.5500000000000002E-3</v>
       </c>
       <c r="D22" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -800,10 +812,10 @@
         <v>32</v>
       </c>
       <c r="B23">
-        <v>441238</v>
+        <v>1191.8</v>
       </c>
       <c r="C23">
-        <v>2.5500000000000002E-3</v>
+        <v>0.86</v>
       </c>
       <c r="D23" t="s">
         <v>10</v>
@@ -811,99 +823,141 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B24">
-        <v>1191.8</v>
+        <v>2341.8000000000002</v>
       </c>
       <c r="C24">
-        <v>0.86</v>
+        <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B25">
-        <v>2341.8000000000002</v>
+        <v>42.56</v>
       </c>
       <c r="C25">
-        <v>1</v>
+        <v>46</v>
       </c>
       <c r="D25" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B26">
-        <v>42.56</v>
+        <v>68.66</v>
       </c>
       <c r="C26">
-        <v>46</v>
+        <v>8</v>
       </c>
       <c r="D26" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B27">
-        <v>68.66</v>
+        <v>941.6</v>
       </c>
       <c r="C27">
-        <v>8</v>
+        <v>1.7</v>
       </c>
       <c r="D27" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B28">
-        <v>621</v>
+        <v>77.5</v>
       </c>
       <c r="C28">
-        <v>1.7</v>
+        <v>19</v>
       </c>
       <c r="D28" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B29">
-        <v>27.5</v>
+        <v>1232</v>
       </c>
       <c r="C29">
-        <v>19</v>
+        <v>0.435</v>
       </c>
       <c r="D29" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30">
+        <v>30.67</v>
+      </c>
+      <c r="C30">
+        <v>37.6</v>
+      </c>
+      <c r="D30" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>42</v>
       </c>
-      <c r="B30">
-        <v>1232</v>
-      </c>
-      <c r="C30">
-        <v>0.435</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="B31">
+        <v>52</v>
+      </c>
+      <c r="C31">
+        <v>3.99</v>
+      </c>
+      <c r="D31" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32">
+        <v>3884</v>
+      </c>
+      <c r="C32">
+        <v>0.123</v>
+      </c>
+      <c r="D32" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>46</v>
+      </c>
+      <c r="B33">
+        <v>1787</v>
+      </c>
+      <c r="C33">
+        <v>0.307</v>
+      </c>
+      <c r="D33" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
small tweak for FORT-USD
</commit_message>
<xml_diff>
--- a/crassets.xlsx
+++ b/crassets.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -490,16 +490,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="105" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -513,7 +513,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -527,7 +527,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -541,7 +541,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -555,7 +555,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -569,7 +569,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -583,7 +583,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -597,7 +597,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -611,7 +611,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -625,7 +625,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -639,7 +639,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -653,7 +653,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -667,7 +667,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -681,7 +681,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -695,7 +695,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -709,7 +709,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>43</v>
       </c>
@@ -723,7 +723,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>44</v>
       </c>
@@ -737,7 +737,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -751,7 +751,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -765,7 +765,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -779,7 +779,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -793,7 +793,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -807,7 +807,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>32</v>
       </c>
@@ -821,7 +821,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -835,7 +835,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -849,7 +849,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>35</v>
       </c>
@@ -863,7 +863,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>36</v>
       </c>
@@ -877,7 +877,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>37</v>
       </c>
@@ -891,7 +891,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>38</v>
       </c>
@@ -905,7 +905,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>39</v>
       </c>
@@ -919,7 +919,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>42</v>
       </c>
@@ -933,7 +933,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>45</v>
       </c>
@@ -947,15 +947,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>46</v>
       </c>
       <c r="B33">
-        <v>1787</v>
+        <v>3822</v>
       </c>
       <c r="C33">
-        <v>0.307</v>
+        <v>0.28599999999999998</v>
       </c>
       <c r="D33" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
update to get data from coingecko if yahoo not working
</commit_message>
<xml_diff>
--- a/crassets.xlsx
+++ b/crassets.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
   <si>
     <t>Name</t>
   </si>
@@ -123,9 +123,6 @@
   </si>
   <si>
     <t>Meme</t>
-  </si>
-  <si>
-    <t>BANANA</t>
   </si>
   <si>
     <t>RAY</t>
@@ -470,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="105" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="105" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,7 +497,7 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>64.900000000000006</v>
+        <v>72.2</v>
       </c>
       <c r="C2">
         <v>145</v>
@@ -581,13 +578,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8">
-        <v>3319</v>
+        <v>4075</v>
       </c>
       <c r="C8">
-        <v>1.03</v>
+        <v>1.4</v>
       </c>
       <c r="D8" t="s">
         <v>21</v>
@@ -623,167 +620,167 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B11">
-        <v>26</v>
+        <v>56240</v>
       </c>
       <c r="C11">
-        <v>61.65</v>
+        <v>0.08</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B12">
-        <v>56240</v>
+        <v>228</v>
       </c>
       <c r="C12">
-        <v>0.08</v>
+        <v>0.49399999999999999</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B13">
-        <v>228</v>
+        <v>7677</v>
       </c>
       <c r="C13">
-        <v>0.49399999999999999</v>
+        <v>1.25</v>
       </c>
       <c r="D13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B14">
-        <v>7677</v>
+        <v>2341.8000000000002</v>
       </c>
       <c r="C14">
-        <v>1.25</v>
+        <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B15">
-        <v>2341.8000000000002</v>
+        <v>476.87</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>9.5</v>
       </c>
       <c r="D15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B16">
-        <v>476.87</v>
+        <v>269.7</v>
       </c>
       <c r="C16">
-        <v>9.5</v>
+        <v>9.4</v>
       </c>
       <c r="D16" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B17">
-        <v>269.7</v>
+        <v>30.67</v>
       </c>
       <c r="C17">
-        <v>9.4</v>
+        <v>37.6</v>
       </c>
       <c r="D17" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B18">
-        <v>30.67</v>
+        <v>14531</v>
       </c>
       <c r="C18">
-        <v>37.6</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="D18" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B19">
-        <v>14531</v>
+        <v>185.18</v>
       </c>
       <c r="C19">
-        <v>7.0000000000000007E-2</v>
+        <v>16</v>
       </c>
       <c r="D19" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B20">
-        <v>185.18</v>
+        <v>3161</v>
       </c>
       <c r="C20">
-        <v>16</v>
+        <v>1.5</v>
       </c>
       <c r="D20" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B21">
-        <v>3161</v>
+        <v>5903</v>
       </c>
       <c r="C21">
-        <v>1.5</v>
+        <v>1.0609999999999999</v>
       </c>
       <c r="D21" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B22">
-        <v>5903</v>
+        <v>300</v>
       </c>
       <c r="C22">
-        <v>1.0609999999999999</v>
+        <v>4.3499999999999996</v>
       </c>
       <c r="D22" t="s">
         <v>4</v>
@@ -791,16 +788,16 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B23">
-        <v>710</v>
+        <v>3153</v>
       </c>
       <c r="C23">
-        <v>4.3499999999999996</v>
+        <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -808,13 +805,13 @@
         <v>35</v>
       </c>
       <c r="B24">
-        <v>3153</v>
+        <v>98839</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="D24" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -822,13 +819,13 @@
         <v>36</v>
       </c>
       <c r="B25">
-        <v>98839</v>
+        <v>775</v>
       </c>
       <c r="C25">
-        <v>8.0000000000000002E-3</v>
+        <v>1.4</v>
       </c>
       <c r="D25" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -836,13 +833,13 @@
         <v>37</v>
       </c>
       <c r="B26">
-        <v>775</v>
+        <v>1852</v>
       </c>
       <c r="C26">
-        <v>1.4</v>
+        <v>1.1339999999999999</v>
       </c>
       <c r="D26" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -850,27 +847,13 @@
         <v>38</v>
       </c>
       <c r="B27">
-        <v>862.35</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="C27">
-        <v>1.2170000000000001</v>
+        <v>45000</v>
       </c>
       <c r="D27" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
         <v>39</v>
-      </c>
-      <c r="B28">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="C28">
-        <v>45000</v>
-      </c>
-      <c r="D28" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
various errors fixed, new versoin yfinance, ohcl still not perfect
</commit_message>
<xml_diff>
--- a/crassets.xlsx
+++ b/crassets.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
   <si>
     <t>Name</t>
   </si>
@@ -62,9 +62,6 @@
     <t>Oracle</t>
   </si>
   <si>
-    <t>ONT</t>
-  </si>
-  <si>
     <t>AAVE</t>
   </si>
   <si>
@@ -128,9 +125,6 @@
     <t>RAY</t>
   </si>
   <si>
-    <t>MPL</t>
-  </si>
-  <si>
     <t>RWA</t>
   </si>
   <si>
@@ -150,6 +144,9 @@
   </si>
   <si>
     <t>Digital Gold</t>
+  </si>
+  <si>
+    <t>AIOZ</t>
   </si>
 </sst>
 </file>
@@ -467,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="105" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="105" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,97 +536,97 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>1643</v>
+        <v>12.08</v>
       </c>
       <c r="C5">
-        <v>1.1000000000000001</v>
+        <v>66.3</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B6">
-        <v>12.08</v>
+        <v>369</v>
       </c>
       <c r="C6">
-        <v>66.3</v>
+        <v>16.600000000000001</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B7">
-        <v>369</v>
+        <v>4075</v>
       </c>
       <c r="C7">
-        <v>16.600000000000001</v>
+        <v>1.4</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B8">
-        <v>4075</v>
+        <v>6367</v>
       </c>
       <c r="C8">
-        <v>1.4</v>
+        <v>0.25290000000000001</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B9">
-        <v>6367</v>
+        <v>239926</v>
       </c>
       <c r="C9">
-        <v>0.25290000000000001</v>
+        <v>1.7729999999999999E-2</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B10">
-        <v>239926</v>
+        <v>56240</v>
       </c>
       <c r="C10">
-        <v>1.7729999999999999E-2</v>
+        <v>0.08</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B11">
-        <v>56240</v>
+        <v>228</v>
       </c>
       <c r="C11">
-        <v>0.08</v>
+        <v>0.49399999999999999</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -637,10 +634,10 @@
         <v>15</v>
       </c>
       <c r="B12">
-        <v>228</v>
+        <v>7677</v>
       </c>
       <c r="C12">
-        <v>0.49399999999999999</v>
+        <v>1.25</v>
       </c>
       <c r="D12" t="s">
         <v>13</v>
@@ -651,13 +648,13 @@
         <v>16</v>
       </c>
       <c r="B13">
-        <v>7677</v>
+        <v>2341.8000000000002</v>
       </c>
       <c r="C13">
-        <v>1.25</v>
+        <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -665,10 +662,10 @@
         <v>17</v>
       </c>
       <c r="B14">
-        <v>2341.8000000000002</v>
+        <v>476.87</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>9.5</v>
       </c>
       <c r="D14" t="s">
         <v>12</v>
@@ -679,13 +676,13 @@
         <v>18</v>
       </c>
       <c r="B15">
-        <v>476.87</v>
+        <v>269.7</v>
       </c>
       <c r="C15">
-        <v>9.5</v>
+        <v>9.4</v>
       </c>
       <c r="D15" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -693,97 +690,97 @@
         <v>19</v>
       </c>
       <c r="B16">
-        <v>269.7</v>
+        <v>30.67</v>
       </c>
       <c r="C16">
-        <v>9.4</v>
+        <v>37.6</v>
       </c>
       <c r="D16" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B17">
-        <v>30.67</v>
+        <v>14531</v>
       </c>
       <c r="C17">
-        <v>37.6</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="D17" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B18">
-        <v>14531</v>
+        <v>3161</v>
       </c>
       <c r="C18">
-        <v>7.0000000000000007E-2</v>
+        <v>1.5</v>
       </c>
       <c r="D18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B19">
-        <v>185.18</v>
+        <v>5903</v>
       </c>
       <c r="C19">
-        <v>16</v>
+        <v>1.0609999999999999</v>
       </c>
       <c r="D19" t="s">
-        <v>33</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B20">
-        <v>3161</v>
+        <v>300</v>
       </c>
       <c r="C20">
-        <v>1.5</v>
+        <v>4.3499999999999996</v>
       </c>
       <c r="D20" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B21">
-        <v>5903</v>
+        <v>3153</v>
       </c>
       <c r="C21">
-        <v>1.0609999999999999</v>
+        <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B22">
-        <v>300</v>
+        <v>98839</v>
       </c>
       <c r="C22">
-        <v>4.3499999999999996</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="D22" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -791,13 +788,13 @@
         <v>34</v>
       </c>
       <c r="B23">
-        <v>3153</v>
+        <v>775</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>1.4</v>
       </c>
       <c r="D23" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -805,13 +802,13 @@
         <v>35</v>
       </c>
       <c r="B24">
-        <v>98839</v>
+        <v>3073</v>
       </c>
       <c r="C24">
-        <v>8.0000000000000002E-3</v>
+        <v>1.04</v>
       </c>
       <c r="D24" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -819,41 +816,27 @@
         <v>36</v>
       </c>
       <c r="B25">
-        <v>775</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="C25">
-        <v>1.4</v>
+        <v>45000</v>
       </c>
       <c r="D25" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B26">
-        <v>1852</v>
+        <v>4621</v>
       </c>
       <c r="C26">
-        <v>1.1339999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="D26" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>38</v>
-      </c>
-      <c r="B27">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="C27">
-        <v>45000</v>
-      </c>
-      <c r="D27" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>